<commit_message>
add new files on EMG features and muscle synergy
</commit_message>
<xml_diff>
--- a/DATA/Patients_Information.xlsx
+++ b/DATA/Patients_Information.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15990" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="8376"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="136">
   <si>
     <t>姓名</t>
   </si>
@@ -307,18 +307,168 @@
   </si>
   <si>
     <t>本院员工</t>
+  </si>
+  <si>
+    <t>倪醒钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>右</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>38分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王晓华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>46分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朱玉江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>右</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公务员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>33分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上肢Brunnstrom分级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手Brunnstrom分级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>III-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IV-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>III+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肌张力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屈肘高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屈肘屈腕高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屈伸肘高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伸肘高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -327,7 +477,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -349,23 +499,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -380,14 +515,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -686,6 +818,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -718,24 +851,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:K46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A31" sqref="$A31:$XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="8.875" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="12.75" customWidth="1"/>
-    <col min="9" max="10" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="9" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -769,8 +901,17 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -804,8 +945,17 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -840,7 +990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="7:11">
+    <row r="4" spans="1:14">
       <c r="G4" s="1">
         <v>41472</v>
       </c>
@@ -851,7 +1001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -877,8 +1027,17 @@
       <c r="K5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" t="s">
+        <v>120</v>
+      </c>
+      <c r="N5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -912,8 +1071,17 @@
       <c r="K6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -947,8 +1115,17 @@
       <c r="K7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7" t="s">
+        <v>120</v>
+      </c>
+      <c r="N7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -982,8 +1159,11 @@
       <c r="K8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="N8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1008,8 +1188,17 @@
       <c r="K9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M9" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1043,8 +1232,17 @@
       <c r="K10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1075,8 +1273,17 @@
       <c r="K11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" t="s">
+        <v>119</v>
+      </c>
+      <c r="M11" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1101,8 +1308,17 @@
       <c r="K12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" t="s">
+        <v>131</v>
+      </c>
+      <c r="M12" t="s">
+        <v>120</v>
+      </c>
+      <c r="N12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1136,8 +1352,17 @@
       <c r="K13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" t="s">
+        <v>124</v>
+      </c>
+      <c r="M13" t="s">
+        <v>131</v>
+      </c>
+      <c r="N13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1171,8 +1396,17 @@
       <c r="K14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" t="s">
+        <v>120</v>
+      </c>
+      <c r="M14" t="s">
+        <v>120</v>
+      </c>
+      <c r="N14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1206,8 +1440,17 @@
       <c r="K15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" t="s">
+        <v>124</v>
+      </c>
+      <c r="M15" t="s">
+        <v>131</v>
+      </c>
+      <c r="N15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1241,8 +1484,17 @@
       <c r="K16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" t="s">
+        <v>124</v>
+      </c>
+      <c r="M16" t="s">
+        <v>120</v>
+      </c>
+      <c r="N16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1253,48 +1505,51 @@
       <c r="K17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="N17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="1">
+        <v>42054</v>
+      </c>
+      <c r="G18" s="1">
+        <v>42123</v>
+      </c>
+      <c r="K18" t="s">
+        <v>107</v>
+      </c>
+      <c r="L18" t="s">
+        <v>124</v>
+      </c>
+      <c r="M18" t="s">
+        <v>125</v>
+      </c>
+      <c r="N18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="1">
-        <v>41725</v>
-      </c>
-      <c r="G18" s="1">
-        <v>41783</v>
-      </c>
-      <c r="H18">
-        <v>63514966</v>
-      </c>
-      <c r="I18" s="1">
-        <v>15958</v>
-      </c>
-      <c r="J18" s="1">
-        <v>41780</v>
-      </c>
-      <c r="K18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19">
-        <v>64</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1306,146 +1561,190 @@
         <v>14</v>
       </c>
       <c r="F19" s="1">
+        <v>41725</v>
+      </c>
+      <c r="G19" s="1">
+        <v>41783</v>
+      </c>
+      <c r="H19">
+        <v>63514966</v>
+      </c>
+      <c r="I19" s="1">
+        <v>15958</v>
+      </c>
+      <c r="J19" s="1">
+        <v>41780</v>
+      </c>
+      <c r="K19" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" t="s">
+        <v>131</v>
+      </c>
+      <c r="N19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="1">
+        <v>42053</v>
+      </c>
+      <c r="G20" s="1">
+        <v>42170</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" t="s">
+        <v>114</v>
+      </c>
+      <c r="L20" t="s">
+        <v>124</v>
+      </c>
+      <c r="M20" t="s">
+        <v>124</v>
+      </c>
+      <c r="N20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1">
         <v>41459</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G21" s="1">
         <v>41569</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>13901093648</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J21" s="1">
         <v>41556</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="7:11">
-      <c r="G20" s="1">
+      <c r="L21" t="s">
+        <v>119</v>
+      </c>
+      <c r="M21" t="s">
+        <v>117</v>
+      </c>
+      <c r="N21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="G22" s="1">
         <v>41592</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J22" s="1">
         <v>41585</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K22" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="7:11">
-      <c r="G21" s="1">
+      <c r="L22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M22" t="s">
+        <v>117</v>
+      </c>
+      <c r="N22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="G23" s="1">
         <v>41604</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J23" s="1">
         <v>41585</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
+      <c r="L23" t="s">
+        <v>119</v>
+      </c>
+      <c r="M23" t="s">
+        <v>117</v>
+      </c>
+      <c r="N23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>29</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>13</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22">
+      <c r="G24" s="1"/>
+      <c r="H24">
         <v>13051265548</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I24" s="1">
         <v>10815</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J24" s="1">
         <v>41233</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
+      <c r="N24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="1">
-        <v>41857</v>
-      </c>
-      <c r="G23" s="1">
-        <v>41873</v>
-      </c>
-      <c r="H23">
-        <v>13954689782</v>
-      </c>
-      <c r="I23" s="1">
-        <v>23942</v>
-      </c>
-      <c r="J23" s="1">
-        <v>41862</v>
-      </c>
-      <c r="K23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="1">
-        <v>41250</v>
-      </c>
-      <c r="H24">
-        <v>13520550092</v>
-      </c>
-      <c r="I24" s="1">
-        <v>20449</v>
-      </c>
-      <c r="J24" s="1">
-        <v>41240</v>
-      </c>
-      <c r="K24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25">
-        <v>66</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -1454,44 +1753,77 @@
         <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="F25" s="1">
-        <v>41944</v>
+        <v>41857</v>
       </c>
       <c r="G25" s="1">
-        <v>41983</v>
+        <v>41873</v>
       </c>
       <c r="H25">
-        <v>13910740520</v>
+        <v>13954689782</v>
       </c>
       <c r="I25" s="1">
-        <v>17513</v>
+        <v>23942</v>
       </c>
       <c r="J25" s="1">
-        <v>41978</v>
+        <v>41862</v>
       </c>
       <c r="K25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="6:11">
-      <c r="F26" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="L25" t="s">
+        <v>119</v>
+      </c>
+      <c r="M25" t="s">
+        <v>117</v>
+      </c>
+      <c r="N25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>59</v>
+      </c>
       <c r="G26" s="1">
-        <v>42028</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+        <v>41250</v>
+      </c>
+      <c r="H26">
+        <v>13520550092</v>
+      </c>
+      <c r="I26" s="1">
+        <v>20449</v>
+      </c>
+      <c r="J26" s="1">
+        <v>41240</v>
+      </c>
       <c r="K26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>60</v>
+      </c>
+      <c r="N26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1500,426 +1832,491 @@
         <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>65</v>
+        <v>14</v>
+      </c>
+      <c r="F27" s="1">
+        <v>41944</v>
+      </c>
+      <c r="G27" s="1">
+        <v>41983</v>
       </c>
       <c r="H27">
-        <v>15811032032</v>
+        <v>13910740520</v>
       </c>
       <c r="I27" s="1">
-        <v>15951</v>
+        <v>17513</v>
       </c>
       <c r="J27" s="1">
-        <v>41416</v>
+        <v>41978</v>
       </c>
       <c r="K27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28">
-        <v>68</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="1">
-        <v>41387</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28">
-        <v>13552119715</v>
-      </c>
-      <c r="I28" s="1">
-        <v>16341</v>
-      </c>
-      <c r="J28" s="1">
-        <v>41386</v>
-      </c>
+      <c r="L27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M27" t="s">
+        <v>122</v>
+      </c>
+      <c r="N27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <v>42028</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
       <c r="K28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>53</v>
+      </c>
+      <c r="L28" t="s">
+        <v>123</v>
+      </c>
+      <c r="M28" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B29">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="1">
-        <v>41905</v>
-      </c>
-      <c r="G29" s="1">
-        <v>42093</v>
+        <v>64</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29">
+        <v>15811032032</v>
+      </c>
+      <c r="I29" s="1">
+        <v>15951</v>
+      </c>
+      <c r="J29" s="1">
+        <v>41416</v>
       </c>
       <c r="K29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>62</v>
+      </c>
+      <c r="L29" t="s">
+        <v>122</v>
+      </c>
+      <c r="N29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="B30">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F30" s="1">
-        <v>41789</v>
+        <v>42076</v>
       </c>
       <c r="G30" s="1">
-        <v>41944</v>
+        <v>42102</v>
       </c>
       <c r="H30">
-        <v>13651032504</v>
-      </c>
-      <c r="I30" s="1">
-        <v>27980</v>
-      </c>
+        <v>13910766773</v>
+      </c>
+      <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M30" t="s">
+        <v>118</v>
+      </c>
+      <c r="N30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="G31" s="1">
+        <v>42115</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" t="s">
+        <v>102</v>
+      </c>
+      <c r="L31" t="s">
+        <v>119</v>
+      </c>
+      <c r="M31" t="s">
+        <v>117</v>
+      </c>
+      <c r="N31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="G32" s="1">
+        <v>42153</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" t="s">
+        <v>108</v>
+      </c>
+      <c r="L32" t="s">
+        <v>120</v>
+      </c>
+      <c r="M32" t="s">
+        <v>121</v>
+      </c>
+      <c r="N32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="1">
+        <v>41387</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33">
+        <v>13552119715</v>
+      </c>
+      <c r="I33" s="1">
+        <v>16341</v>
+      </c>
+      <c r="J33" s="1">
+        <v>41386</v>
+      </c>
+      <c r="K33" t="s">
+        <v>67</v>
+      </c>
+      <c r="L33" t="s">
+        <v>117</v>
+      </c>
+      <c r="N33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
         <v>13</v>
       </c>
-      <c r="E31" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="1">
-        <v>42031</v>
-      </c>
-      <c r="G31" s="1">
-        <v>42095</v>
-      </c>
-      <c r="K31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32">
-        <v>54</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="E34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="1">
+        <v>41905</v>
+      </c>
+      <c r="G34" s="1">
+        <v>42093</v>
+      </c>
+      <c r="K34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L34" t="s">
+        <v>122</v>
+      </c>
+      <c r="M34" t="s">
+        <v>118</v>
+      </c>
+      <c r="N34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1">
+        <v>42153</v>
+      </c>
+      <c r="K35" t="s">
+        <v>110</v>
+      </c>
+      <c r="L35" t="s">
+        <v>123</v>
+      </c>
+      <c r="M35" t="s">
+        <v>118</v>
+      </c>
+      <c r="N35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
         <v>12</v>
       </c>
-      <c r="E32" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="1">
-        <v>41460</v>
-      </c>
-      <c r="H32">
-        <v>13701277672</v>
-      </c>
-      <c r="I32" s="1">
-        <v>21419</v>
-      </c>
-      <c r="J32" s="1">
-        <v>41451</v>
-      </c>
-      <c r="K32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="1">
-        <v>41398</v>
-      </c>
-      <c r="G33" s="1">
-        <v>41460</v>
-      </c>
-      <c r="K33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="7:11">
-      <c r="G34" s="1">
-        <v>41494</v>
-      </c>
-      <c r="K34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35">
-        <v>63</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>18</v>
       </c>
-      <c r="E35" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="1">
-        <v>41305</v>
-      </c>
-      <c r="G35" s="1">
-        <v>41362</v>
-      </c>
-      <c r="H35">
-        <v>13511059973</v>
-      </c>
-      <c r="I35" s="1">
-        <v>18523</v>
-      </c>
-      <c r="J35" s="1">
-        <v>41360</v>
-      </c>
-      <c r="K35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="7:11">
+      <c r="E36" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="1">
+        <v>41789</v>
+      </c>
       <c r="G36" s="1">
-        <v>41387</v>
-      </c>
-      <c r="J36" s="1">
-        <v>41374</v>
-      </c>
+        <v>41944</v>
+      </c>
+      <c r="H36">
+        <v>13651032504</v>
+      </c>
+      <c r="I36" s="1">
+        <v>27980</v>
+      </c>
+      <c r="J36" s="1"/>
       <c r="K36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" t="s">
+        <v>122</v>
+      </c>
+      <c r="M36" t="s">
+        <v>117</v>
+      </c>
+      <c r="N36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="1">
+        <v>42031</v>
+      </c>
+      <c r="G37" s="1">
+        <v>42095</v>
+      </c>
+      <c r="K37" t="s">
+        <v>71</v>
+      </c>
+      <c r="L37" t="s">
+        <v>122</v>
+      </c>
+      <c r="M37" t="s">
+        <v>118</v>
+      </c>
+      <c r="N37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1">
+        <v>42170</v>
+      </c>
+      <c r="K38" t="s">
+        <v>109</v>
+      </c>
+      <c r="L38" t="s">
+        <v>119</v>
+      </c>
+      <c r="M38" t="s">
+        <v>117</v>
+      </c>
+      <c r="N38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>75</v>
+      </c>
+      <c r="G39" s="1">
+        <v>41460</v>
+      </c>
+      <c r="H39">
+        <v>13701277672</v>
+      </c>
+      <c r="I39" s="1">
+        <v>21419</v>
+      </c>
+      <c r="J39" s="1">
+        <v>41451</v>
+      </c>
+      <c r="K39" t="s">
+        <v>71</v>
+      </c>
+      <c r="N39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="1">
+        <v>41398</v>
+      </c>
+      <c r="G40" s="1">
+        <v>41460</v>
+      </c>
+      <c r="K40" t="s">
+        <v>71</v>
+      </c>
+      <c r="L40" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="G41" s="1">
+        <v>41494</v>
+      </c>
+      <c r="K41" t="s">
+        <v>62</v>
+      </c>
+      <c r="L41" t="s">
+        <v>122</v>
+      </c>
+      <c r="N41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="1">
+        <v>41305</v>
+      </c>
+      <c r="G42" s="1">
+        <v>41362</v>
+      </c>
+      <c r="H42">
+        <v>13511059973</v>
+      </c>
+      <c r="I42" s="1">
+        <v>18523</v>
+      </c>
+      <c r="J42" s="1">
+        <v>41360</v>
+      </c>
+      <c r="K42" t="s">
+        <v>79</v>
+      </c>
+      <c r="N42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="G43" s="1">
+        <v>41387</v>
+      </c>
+      <c r="J43" s="1">
+        <v>41374</v>
+      </c>
+      <c r="K43" t="s">
+        <v>71</v>
+      </c>
+      <c r="N43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
         <v>80</v>
       </c>
-      <c r="B37">
+      <c r="B44">
         <v>53</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" s="1">
-        <v>41319</v>
-      </c>
-      <c r="G37" s="1">
-        <v>41352</v>
-      </c>
-      <c r="H37">
-        <v>18618285639</v>
-      </c>
-      <c r="I37" s="1">
-        <v>41323</v>
-      </c>
-      <c r="J37" s="1">
-        <v>41339</v>
-      </c>
-      <c r="K37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38">
-        <v>79</v>
-      </c>
-      <c r="C38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" s="1">
-        <v>41774</v>
-      </c>
-      <c r="G38" s="1">
-        <v>41832</v>
-      </c>
-      <c r="H38">
-        <v>13439836254</v>
-      </c>
-      <c r="I38" s="1">
-        <v>12917</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39">
-        <v>48</v>
-      </c>
-      <c r="C39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="1">
-        <v>41776</v>
-      </c>
-      <c r="G39" s="1">
-        <v>41832</v>
-      </c>
-      <c r="H39">
-        <v>15910992431</v>
-      </c>
-      <c r="I39" s="1">
-        <v>24292</v>
-      </c>
-      <c r="J39" s="1">
-        <v>41828</v>
-      </c>
-      <c r="K39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="7:11">
-      <c r="G40" s="1">
-        <v>41853</v>
-      </c>
-      <c r="J40" s="1">
-        <v>41844</v>
-      </c>
-      <c r="K40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41">
-        <v>62</v>
-      </c>
-      <c r="C41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G41" s="1">
-        <v>41579</v>
-      </c>
-      <c r="H41">
-        <v>13901235676</v>
-      </c>
-      <c r="I41" s="1">
-        <v>25355</v>
-      </c>
-      <c r="J41" s="1">
-        <v>41575</v>
-      </c>
-      <c r="K41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="7:11">
-      <c r="G42" s="1">
-        <v>41612</v>
-      </c>
-      <c r="J42" s="1">
-        <v>41612</v>
-      </c>
-      <c r="K42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="7:11">
-      <c r="G43" s="1">
-        <v>41649</v>
-      </c>
-      <c r="J43" s="1">
-        <v>41631</v>
-      </c>
-      <c r="K43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B44">
-        <v>64</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
@@ -1928,104 +2325,355 @@
         <v>18</v>
       </c>
       <c r="E44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="1">
+        <v>41319</v>
+      </c>
+      <c r="G44" s="1">
+        <v>41352</v>
+      </c>
+      <c r="H44">
+        <v>18618285639</v>
+      </c>
+      <c r="I44" s="1">
+        <v>41323</v>
+      </c>
+      <c r="J44" s="1">
+        <v>41339</v>
+      </c>
+      <c r="K44" t="s">
+        <v>82</v>
+      </c>
+      <c r="L44" t="s">
+        <v>117</v>
+      </c>
+      <c r="N44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="1">
+        <v>41774</v>
+      </c>
+      <c r="G45" s="1">
+        <v>41832</v>
+      </c>
+      <c r="H45">
+        <v>13439836254</v>
+      </c>
+      <c r="I45" s="1">
+        <v>12917</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K45" t="s">
+        <v>86</v>
+      </c>
+      <c r="L45" t="s">
+        <v>118</v>
+      </c>
+      <c r="M45" t="s">
+        <v>118</v>
+      </c>
+      <c r="N45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="1">
+        <v>41776</v>
+      </c>
+      <c r="G46" s="1">
+        <v>41832</v>
+      </c>
+      <c r="H46">
+        <v>15910992431</v>
+      </c>
+      <c r="I46" s="1">
+        <v>24292</v>
+      </c>
+      <c r="J46" s="1">
+        <v>41828</v>
+      </c>
+      <c r="K46" t="s">
+        <v>86</v>
+      </c>
+      <c r="L46" t="s">
+        <v>122</v>
+      </c>
+      <c r="M46" t="s">
+        <v>132</v>
+      </c>
+      <c r="N46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="G47" s="1">
+        <v>41853</v>
+      </c>
+      <c r="J47" s="1">
+        <v>41844</v>
+      </c>
+      <c r="K47" t="s">
+        <v>86</v>
+      </c>
+      <c r="L47" t="s">
+        <v>122</v>
+      </c>
+      <c r="M47" t="s">
+        <v>117</v>
+      </c>
+      <c r="N47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
         <v>14</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48" s="1">
+        <v>41579</v>
+      </c>
+      <c r="H48">
+        <v>13901235676</v>
+      </c>
+      <c r="I48" s="1">
+        <v>25355</v>
+      </c>
+      <c r="J48" s="1">
+        <v>41575</v>
+      </c>
+      <c r="K48" t="s">
+        <v>86</v>
+      </c>
+      <c r="L48" t="s">
+        <v>117</v>
+      </c>
+      <c r="M48" t="s">
+        <v>132</v>
+      </c>
+      <c r="N48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="G49" s="1">
+        <v>41612</v>
+      </c>
+      <c r="J49" s="1">
+        <v>41612</v>
+      </c>
+      <c r="K49" t="s">
+        <v>71</v>
+      </c>
+      <c r="L49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M49" t="s">
+        <v>122</v>
+      </c>
+      <c r="N49" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="G50" s="1">
+        <v>41649</v>
+      </c>
+      <c r="J50" s="1">
+        <v>41631</v>
+      </c>
+      <c r="K50" t="s">
+        <v>91</v>
+      </c>
+      <c r="L50" t="s">
+        <v>119</v>
+      </c>
+      <c r="M50" t="s">
+        <v>119</v>
+      </c>
+      <c r="N50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51">
+        <v>64</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="1">
         <v>41909</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G51" s="1">
         <v>41936</v>
       </c>
-      <c r="H44">
+      <c r="H51">
         <v>13001907537</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I51" s="1">
         <v>18267</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J51" s="1">
         <v>41935</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="7:11">
-      <c r="G45" s="1">
+      <c r="L51" t="s">
+        <v>117</v>
+      </c>
+      <c r="M51" t="s">
+        <v>117</v>
+      </c>
+      <c r="N51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="G52" s="1">
         <v>41948</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J52" s="1">
         <v>41935</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K52" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
+      <c r="L52" t="s">
+        <v>117</v>
+      </c>
+      <c r="M52" t="s">
+        <v>122</v>
+      </c>
+      <c r="N52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
         <v>95</v>
       </c>
-      <c r="B46">
+      <c r="B53">
         <v>84</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D53" t="s">
         <v>13</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E53" t="s">
         <v>96</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F53" s="1">
         <v>41216</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46">
+      <c r="G53" s="1"/>
+      <c r="H53">
         <v>66125658</v>
       </c>
-      <c r="I46">
+      <c r="I53">
         <v>192891</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J53" s="1">
         <v>41219</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K53" t="s">
         <v>93</v>
       </c>
+      <c r="N53" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>